<commit_message>
Ocean Data Lab2 WIP
</commit_message>
<xml_diff>
--- a/Ocean_date.xlsx
+++ b/Ocean_date.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Ocean_date\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unpat\_Projects\Ocean_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E310ECB1-3246-4F42-8D5E-4DB1ED0201D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560532DA-ECD0-48DF-9D2A-0985CE32E6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,15 +101,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -373,7 +364,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -668,7 +659,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +727,7 @@
       </c>
       <c r="F4" s="18">
         <f>SUM(E4:E10)</f>
-        <v>6.2499999999999889E-2</v>
+        <v>0.14583333333333337</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>9</v>
@@ -774,21 +765,30 @@
         <v>0.96875</v>
       </c>
       <c r="D6" s="29">
-        <v>0.94791666666666663</v>
+        <v>0.98958333333333337</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" ref="E6" si="2">D6-C6</f>
-        <v>-2.083333333333337E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="B7" s="8">
+        <v>44868</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" ref="E7" si="3">D7-C7</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
       <c r="F7" s="20"/>
       <c r="G7" s="24"/>
     </row>

</xml_diff>